<commit_message>
Cambiando de LinearRegression a LogisticRegression
</commit_message>
<xml_diff>
--- a/rendimientos.xlsx
+++ b/rendimientos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cdca\Desktop\Performcast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Clases\FLASH MACHINE LEARNING\performcast-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3E5A20F-0583-4E77-85F6-A610721E2D8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EADF871-E38B-498D-B9A4-E2CFC34DB23B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F570A082-FA01-40AB-AA62-2B2EEF6DB5E6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F570A082-FA01-40AB-AA62-2B2EEF6DB5E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -448,21 +448,21 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -485,7 +485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -508,7 +508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7</v>
       </c>
@@ -551,7 +551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -565,7 +565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>15</v>
       </c>
@@ -573,52 +573,52 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
         <v>5</v>
       </c>

</xml_diff>